<commit_message>
Add capturing to report
</commit_message>
<xml_diff>
--- a/report/drivespeeds.xlsx
+++ b/report/drivespeeds.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mineichen/hslu/changeDetectionProject/cameraChangeDetection/report/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -152,18 +160,23 @@
     <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -492,15 +505,16 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1">
         <v>53.035800000000002</v>
       </c>
@@ -513,7 +527,7 @@
         <v>2.96630859375</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>49.799100000000003</v>
       </c>
@@ -522,7 +536,7 @@
         <v>10.281310304804705</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>50.402500000000003</v>
       </c>
@@ -531,7 +545,7 @@
         <v>10.158226278458409</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>51.029600000000002</v>
       </c>
@@ -540,7 +554,7 @@
         <v>10.033392384028094</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>51.089700000000001</v>
       </c>
@@ -549,7 +563,7 @@
         <v>10.021589478896921</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>50.883000000000003</v>
       </c>
@@ -558,7 +572,7 @@
         <v>10.06229978578307</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>51.029600000000002</v>
       </c>
@@ -567,7 +581,7 @@
         <v>10.033392384028094</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>51.089700000000001</v>
       </c>
@@ -576,7 +590,7 @@
         <v>10.021589478896921</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>50.883000000000003</v>
       </c>
@@ -585,12 +599,12 @@
         <v>10.06229978578307</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -602,7 +616,7 @@
         <v>15.098301146232355</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -614,7 +628,7 @@
         <v>16.524764554380031</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -626,7 +640,7 @@
         <v>14.597832564000946</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -638,7 +652,7 @@
         <v>16.831308864379757</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -650,7 +664,7 @@
         <v>16.014813702674974</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -662,7 +676,7 @@
         <v>15.712895929684791</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -678,7 +692,7 @@
         <v>3.2491582491582491</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -694,7 +708,7 @@
         <v>18.665558399136717</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -706,7 +720,7 @@
         <v>16.235722394515371</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -714,7 +728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -738,7 +752,7 @@
         <v>12.136296296296296</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -762,7 +776,7 @@
         <v>10.748722289825935</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -774,7 +788,7 @@
         <v>15.548037971223984</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -786,7 +800,7 @@
         <v>17.472017472017473</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -798,7 +812,7 @@
         <v>16.86085186819556</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -810,7 +824,7 @@
         <v>18.071311087737627</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -822,7 +836,7 @@
         <v>17.545182271141602</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -834,7 +848,7 @@
         <v>17.555890824303937</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -849,10 +863,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>